<commit_message>
base suite- donnée de teste
</commit_message>
<xml_diff>
--- a/Bdd/donnée.xlsx
+++ b/Bdd/donnée.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="348">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -384,6 +384,15 @@
     <t xml:space="preserve">patsa</t>
   </si>
   <si>
+    <t xml:space="preserve">tsatsiou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> canard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chapelure</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maladie</t>
   </si>
   <si>
@@ -588,42 +597,81 @@
     <t xml:space="preserve">Plat</t>
   </si>
   <si>
+    <t xml:space="preserve">recettes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plat Ingredient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mofo akondro</t>
   </si>
   <si>
+    <t xml:space="preserve">5-3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mofo anana</t>
   </si>
   <si>
     <t xml:space="preserve">Mofo baolina</t>
   </si>
   <si>
+    <t xml:space="preserve">05-03-6-</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pakopako</t>
   </si>
   <si>
+    <t xml:space="preserve">5--</t>
+  </si>
+  <si>
     <t xml:space="preserve">Riz cantonais</t>
   </si>
   <si>
+    <t xml:space="preserve">9-10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Riz Firt</t>
   </si>
   <si>
     <t xml:space="preserve">ailes de poulet caramelisé</t>
   </si>
   <si>
+    <t xml:space="preserve">1-3-10-</t>
+  </si>
+  <si>
     <t xml:space="preserve">cuisse de poulet grilé</t>
   </si>
   <si>
+    <t xml:space="preserve">3-10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pistolet</t>
   </si>
   <si>
+    <t xml:space="preserve">3-10-</t>
+  </si>
+  <si>
     <t xml:space="preserve">Poivron farci </t>
   </si>
   <si>
+    <t xml:space="preserve">2-3</t>
+  </si>
+  <si>
     <t xml:space="preserve">hena Omby ritra</t>
   </si>
   <si>
+    <t xml:space="preserve">1-11-4-</t>
+  </si>
+  <si>
     <t xml:space="preserve">tripy sauce</t>
   </si>
   <si>
+    <t xml:space="preserve">1-11</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tsaramaso sy Henakisoa</t>
   </si>
   <si>
@@ -645,12 +693,18 @@
     <t xml:space="preserve">Voatavo sy voanjo </t>
   </si>
   <si>
-    <t xml:space="preserve">Legioma saosy</t>
+    <t xml:space="preserve">Legume sauté</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-9</t>
   </si>
   <si>
     <t xml:space="preserve">Saucisse Fumée sy Legioma</t>
   </si>
   <si>
+    <t xml:space="preserve">1-11-10-</t>
+  </si>
+  <si>
     <t xml:space="preserve">Saucisse Porc sy Tsaramaso</t>
   </si>
   <si>
@@ -678,9 +732,15 @@
     <t xml:space="preserve">Hors d œuvre</t>
   </si>
   <si>
+    <t xml:space="preserve">2-10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Salade de pate</t>
   </si>
   <si>
+    <t xml:space="preserve">2-3-10-</t>
+  </si>
+  <si>
     <t xml:space="preserve">Salade éxotique</t>
   </si>
   <si>
@@ -960,10 +1020,10 @@
     <t xml:space="preserve">Petit Paté</t>
   </si>
   <si>
-    <t xml:space="preserve">Pain au cocho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pain au raison</t>
+    <t xml:space="preserve">Pain au choco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pain au raisin</t>
   </si>
   <si>
     <t xml:space="preserve">Crêpe au chocolat</t>
@@ -997,21 +1057,42 @@
   </si>
   <si>
     <t xml:space="preserve">Vomanga atono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Croquette de Poulet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Croquette de Fromage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1  | plats principaux     |    1
+ 2  | entrée/apéritifs     |    1
+ 3  | snacks               |    1
+ 4  | résistance           |    1
+ 5  | dessert              |    1
+ 6  | petit déjeuner       |    1
+ 7  | plats traditionnels  |    1
+ 8  | soupe                |    1
+ 9  | accompagnement       |    1
+ 10 | plats de fête        |    1
+ 11 | plats trad(Malagasy) |    1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1030,6 +1111,13 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1078,7 +1166,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1092,6 +1180,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1112,13 +1212,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E105" activeCellId="0" sqref="E105"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
@@ -2951,6 +3051,57 @@
       </c>
       <c r="E104" s="0" t="n">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E105" s="0" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D106" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E106" s="0" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D107" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E107" s="0" t="n">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>
@@ -2969,37 +3120,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A63" activeCellId="0" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -3007,7 +3158,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -3016,12 +3167,12 @@
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -3030,12 +3181,12 @@
         <v>2</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
@@ -3044,12 +3195,12 @@
         <v>3</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -3057,7 +3208,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2</v>
@@ -3065,7 +3216,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2</v>
@@ -3073,7 +3224,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>
@@ -3081,7 +3232,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -3089,7 +3240,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -3097,7 +3248,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
@@ -3105,7 +3256,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1</v>
@@ -3113,7 +3264,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -3121,7 +3272,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -3129,7 +3280,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
@@ -3137,7 +3288,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
@@ -3145,7 +3296,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
@@ -3153,7 +3304,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
@@ -3161,7 +3312,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>2</v>
@@ -3169,7 +3320,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
@@ -3177,7 +3328,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -3185,7 +3336,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2</v>
@@ -3193,7 +3344,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>2</v>
@@ -3201,7 +3352,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>2</v>
@@ -3209,7 +3360,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>2</v>
@@ -3217,7 +3368,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>2</v>
@@ -3225,7 +3376,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>2</v>
@@ -3233,7 +3384,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>2</v>
@@ -3241,7 +3392,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>3</v>
@@ -3249,7 +3400,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>3</v>
@@ -3257,7 +3408,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -3265,7 +3416,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
@@ -3273,7 +3424,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
@@ -3281,7 +3432,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
@@ -3289,7 +3440,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
@@ -3297,7 +3448,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
@@ -3305,7 +3456,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -3313,7 +3464,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
@@ -3321,7 +3472,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1</v>
@@ -3329,7 +3480,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
@@ -3337,7 +3488,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
@@ -3345,7 +3496,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1</v>
@@ -3353,7 +3504,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1</v>
@@ -3361,7 +3512,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1</v>
@@ -3369,7 +3520,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
@@ -3377,7 +3528,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>1</v>
@@ -3385,7 +3536,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1</v>
@@ -3393,7 +3544,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>1</v>
@@ -3401,7 +3552,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1</v>
@@ -3409,7 +3560,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>1</v>
@@ -3417,7 +3568,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>1</v>
@@ -3425,7 +3576,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>1</v>
@@ -3433,7 +3584,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
@@ -3441,7 +3592,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>3</v>
@@ -3449,7 +3600,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>3</v>
@@ -3457,7 +3608,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>1</v>
@@ -3465,7 +3616,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>1</v>
@@ -3473,7 +3624,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>1</v>
@@ -3481,7 +3632,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>1</v>
@@ -3489,7 +3640,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>3</v>
@@ -3497,13 +3648,12 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -3520,705 +3670,1337 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:B138"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="35.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>190</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="B2" s="0" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>194</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="B3" s="0" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>196</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="B4" s="0" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>197</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B5" s="0" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>199</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="B6" s="0" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>201</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="B7" s="0" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>203</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="B8" s="0" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>204</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="B9" s="0" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>206</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
       <c r="B10" s="0" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>208</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="B11" s="0" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>210</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
       <c r="B12" s="0" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>212</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
       <c r="B13" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>214</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
       <c r="B14" s="0" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>216</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
       <c r="B15" s="0" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>217</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
       <c r="B16" s="0" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>218</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
       <c r="B17" s="0" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>219</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
       <c r="B18" s="0" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>220</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
       <c r="B19" s="0" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>221</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
       <c r="B20" s="0" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>222</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
       <c r="B21" s="0" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>223</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
       <c r="B22" s="0" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>225</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
       <c r="B23" s="0" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>227</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
       <c r="B24" s="0" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>228</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
       <c r="B25" s="0" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>229</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
       <c r="B26" s="0" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>230</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
       <c r="B27" s="0" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>231</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
       <c r="B28" s="0" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>232</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
       <c r="B29" s="0" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>233</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
       <c r="B30" s="0" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>234</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
       <c r="B31" s="0" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>235</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
       <c r="B32" s="0" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>237</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
       <c r="B33" s="0" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
       <c r="B34" s="0" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
       <c r="B35" s="0" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
       <c r="B36" s="0" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
       <c r="B37" s="0" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
       <c r="B38" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
       <c r="B39" s="0" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
       <c r="B40" s="0" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
       <c r="B41" s="0" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
       <c r="B42" s="0" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
       <c r="B43" s="0" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
       <c r="B44" s="0" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
       <c r="B45" s="0" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
       <c r="B46" s="0" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
       <c r="B47" s="0" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
       <c r="B48" s="0" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
       <c r="B49" s="0" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
       <c r="B50" s="0" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
       <c r="B51" s="0" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>51</v>
+      </c>
       <c r="B52" s="0" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>52</v>
+      </c>
       <c r="B53" s="0" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>53</v>
+      </c>
       <c r="B54" s="0" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>54</v>
+      </c>
       <c r="B55" s="0" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>55</v>
+      </c>
       <c r="B56" s="0" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>56</v>
+      </c>
       <c r="B57" s="0" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>57</v>
+      </c>
       <c r="B58" s="0" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>58</v>
+      </c>
       <c r="B59" s="0" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>59</v>
+      </c>
       <c r="B60" s="0" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>60</v>
+      </c>
       <c r="B61" s="0" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>61</v>
+      </c>
       <c r="B62" s="0" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>62</v>
+      </c>
       <c r="B63" s="0" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>63</v>
+      </c>
       <c r="B64" s="0" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>64</v>
+      </c>
       <c r="B65" s="0" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>65</v>
+      </c>
       <c r="B66" s="0" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>66</v>
+      </c>
       <c r="B67" s="0" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>67</v>
+      </c>
       <c r="B68" s="0" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>68</v>
+      </c>
       <c r="B69" s="0" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>69</v>
+      </c>
       <c r="B70" s="0" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>70</v>
+      </c>
       <c r="B71" s="0" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>71</v>
+      </c>
       <c r="B72" s="0" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>72</v>
+      </c>
       <c r="B73" s="0" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>73</v>
+      </c>
       <c r="B74" s="0" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>74</v>
+      </c>
       <c r="B75" s="0" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>75</v>
+      </c>
       <c r="B76" s="0" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>76</v>
+      </c>
       <c r="B77" s="0" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>77</v>
+      </c>
       <c r="B78" s="0" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>78</v>
+      </c>
       <c r="B79" s="0" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>79</v>
+      </c>
       <c r="B80" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>80</v>
+      </c>
       <c r="B81" s="0" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>81</v>
+      </c>
       <c r="B82" s="0" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>82</v>
+      </c>
       <c r="B83" s="0" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>83</v>
+      </c>
       <c r="B84" s="0" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>84</v>
+      </c>
       <c r="B85" s="0" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>85</v>
+      </c>
       <c r="B86" s="0" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>86</v>
+      </c>
       <c r="B87" s="0" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>87</v>
+      </c>
       <c r="B88" s="0" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>88</v>
+      </c>
       <c r="B89" s="0" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>89</v>
+      </c>
       <c r="B90" s="0" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <v>90</v>
+      </c>
       <c r="B91" s="0" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <v>91</v>
+      </c>
       <c r="B92" s="0" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <v>92</v>
+      </c>
       <c r="B93" s="0" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <v>93</v>
+      </c>
       <c r="B94" s="0" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="n">
+        <v>94</v>
+      </c>
       <c r="B95" s="0" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <v>95</v>
+      </c>
       <c r="B96" s="0" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <v>96</v>
+      </c>
       <c r="B97" s="0" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="n">
+        <v>97</v>
+      </c>
       <c r="B98" s="0" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="n">
+        <v>98</v>
+      </c>
       <c r="B99" s="0" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <v>99</v>
+      </c>
       <c r="B100" s="0" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="B101" s="0" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="n">
+        <v>101</v>
+      </c>
       <c r="B102" s="0" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <v>102</v>
+      </c>
       <c r="B103" s="0" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="n">
+        <v>103</v>
+      </c>
       <c r="B104" s="0" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <v>104</v>
+      </c>
       <c r="B105" s="0" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <v>105</v>
+      </c>
       <c r="B106" s="0" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <v>106</v>
+      </c>
       <c r="B107" s="0" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <v>107</v>
+      </c>
       <c r="B108" s="0" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <v>108</v>
+      </c>
       <c r="B109" s="0" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="n">
+        <v>109</v>
+      </c>
       <c r="B110" s="0" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="n">
+        <v>110</v>
+      </c>
       <c r="B111" s="0" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="n">
+        <v>111</v>
+      </c>
       <c r="B112" s="0" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="n">
+        <v>112</v>
+      </c>
       <c r="B113" s="0" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="n">
+        <v>113</v>
+      </c>
       <c r="B114" s="0" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <v>114</v>
+      </c>
       <c r="B115" s="0" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="n">
+        <v>115</v>
+      </c>
       <c r="B116" s="0" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <v>116</v>
+      </c>
       <c r="B117" s="0" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <v>117</v>
+      </c>
       <c r="B118" s="0" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <v>118</v>
+      </c>
       <c r="B119" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <v>119</v>
+      </c>
       <c r="B120" s="0" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="n">
+        <v>120</v>
+      </c>
       <c r="B121" s="0" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="n">
+        <v>121</v>
+      </c>
       <c r="B122" s="0" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="n">
+        <v>122</v>
+      </c>
       <c r="B123" s="0" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="n">
+        <v>123</v>
+      </c>
       <c r="B124" s="0" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="n">
+        <v>124</v>
+      </c>
       <c r="B125" s="0" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="n">
+        <v>125</v>
+      </c>
       <c r="B126" s="0" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="n">
+        <v>126</v>
+      </c>
       <c r="B127" s="0" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <v>127</v>
+      </c>
       <c r="B128" s="0" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="n">
+        <v>128</v>
+      </c>
       <c r="B129" s="0" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="n">
+        <v>129</v>
+      </c>
       <c r="B130" s="0" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="n">
+        <v>130</v>
+      </c>
       <c r="B131" s="0" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="n">
+        <v>131</v>
+      </c>
       <c r="B132" s="0" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="n">
+        <v>132</v>
+      </c>
       <c r="B133" s="0" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="n">
+        <v>133</v>
+      </c>
       <c r="B134" s="0" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="n">
+        <v>134</v>
+      </c>
       <c r="B135" s="0" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="n">
+        <v>135</v>
+      </c>
       <c r="B136" s="0" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="n">
+        <v>136</v>
+      </c>
       <c r="B137" s="0" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="n">
+        <v>137</v>
+      </c>
       <c r="B138" s="0" t="s">
-        <v>324</v>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="B140" s="0" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H141" s="6" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>